<commit_message>
add some test cases
</commit_message>
<xml_diff>
--- a/src/main/java/com/renpay/config/testdata.xlsx
+++ b/src/main/java/com/renpay/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19356" windowHeight="7872"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19356" windowHeight="7872" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Password</t>
   </si>
@@ -39,9 +39,6 @@
     <t>ValidValues</t>
   </si>
   <si>
-    <t>LoginPage</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -52,6 +49,39 @@
   </si>
   <si>
     <t>Please check the username or password you have entered and also ensure you have selected the right profile – Buyer or Supplier</t>
+  </si>
+  <si>
+    <t>BlankUserName</t>
+  </si>
+  <si>
+    <t>Please enter Email / Mobile Number.</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>InvalidValue</t>
+  </si>
+  <si>
+    <t>InvalidVallue</t>
+  </si>
+  <si>
+    <t>IncorrectUserNameAndPassword</t>
+  </si>
+  <si>
+    <t>InvalidValues</t>
+  </si>
+  <si>
+    <t>You have entered wrong Username / Mobile Number.Please try again or contact us at help@renepay.com.</t>
+  </si>
+  <si>
+    <t>ForgotPasswordInvalidEmail</t>
+  </si>
+  <si>
+    <t>Password reset link has been sent on your registered email id.Please check your registered email account.</t>
+  </si>
+  <si>
+    <t>ForgotPasswordValidEmail</t>
   </si>
 </sst>
 </file>
@@ -392,48 +422,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>9568989975</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -444,16 +484,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -461,28 +501,47 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final commit for demo
</commit_message>
<xml_diff>
--- a/src/main/java/com/renpay/config/testdata.xlsx
+++ b/src/main/java/com/renpay/config/testdata.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19356" windowHeight="7872" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19356" windowHeight="7872" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="1" r:id="rId1"/>
     <sheet name="ErrorMessages" sheetId="2" r:id="rId2"/>
     <sheet name="SignUpPage" sheetId="3" r:id="rId3"/>
+    <sheet name="ProfilePage" sheetId="4" r:id="rId4"/>
+    <sheet name="CreateRFA" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>Password</t>
   </si>
@@ -157,13 +159,64 @@
     <t>AlreadyRegisteredUserErrorMsg</t>
   </si>
   <si>
-    <t>This email already exists on our system. If you have registered before with us, sign in again with this email and click on Forgot Password</t>
-  </si>
-  <si>
     <t>AcceptTermsAndConditionErrorMsg</t>
   </si>
   <si>
     <t>Please accept terms &amp; conditions</t>
+  </si>
+  <si>
+    <t>MaxLengthValue</t>
+  </si>
+  <si>
+    <t>CreateRFPError</t>
+  </si>
+  <si>
+    <t>Please Enter product name.</t>
+  </si>
+  <si>
+    <t>Mineral Water</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>SubCategory</t>
+  </si>
+  <si>
+    <t>Drinking Water,Package,Packaging Machine,Treatment Equipments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travel &amp; Hotels </t>
+  </si>
+  <si>
+    <t>Guest Houses,OYO Rooms ,Travel &amp; Lodging</t>
+  </si>
+  <si>
+    <t>Travel &amp; Hotels</t>
+  </si>
+  <si>
+    <t>SuppliersName</t>
+  </si>
+  <si>
+    <t>ARCHER TOURS PVT LTD</t>
+  </si>
+  <si>
+    <t>SHIVAM ENTERPRISES</t>
+  </si>
+  <si>
+    <t>CreateRFPSupplierError</t>
+  </si>
+  <si>
+    <t>Please select atleast one supplier.</t>
+  </si>
+  <si>
+    <t>Ajay</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>Company Name Already Exists. Please try With Different Name.</t>
   </si>
 </sst>
 </file>
@@ -579,10 +632,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,15 +705,36 @@
         <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
         <v>44</v>
       </c>
-      <c r="B9" t="s">
-        <v>45</v>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -673,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,6 +776,9 @@
       <c r="B2" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -710,6 +787,9 @@
       <c r="B3" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -718,6 +798,9 @@
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -726,6 +809,9 @@
       <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -734,6 +820,9 @@
       <c r="B6" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -742,6 +831,9 @@
       <c r="B7" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -750,6 +842,9 @@
       <c r="B8" s="2">
         <v>201301</v>
       </c>
+      <c r="C8" s="2">
+        <v>201301</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -758,6 +853,9 @@
       <c r="B9" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -766,6 +864,9 @@
       <c r="B10" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="C10" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -774,6 +875,9 @@
       <c r="B11" s="2">
         <v>9568989975</v>
       </c>
+      <c r="C11" s="2">
+        <v>9568989975</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -782,11 +886,112 @@
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="C10" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>